<commit_message>
first finished version of Python notebook
</commit_message>
<xml_diff>
--- a/fundamental/L-S_small_example.xlsx
+++ b/fundamental/L-S_small_example.xlsx
@@ -5,19 +5,16 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\p_h_d\Dropbox\2-TEACHING\000 - LSMC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\p_h_d\Dropbox\2-TEACHING\000 - LSMC\SUPER_LSMC\fundamental\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B168F4A-4DAB-4913-A99F-2A0EE67FB525}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97348F2B-BAB3-4636-905B-32B4F892ECDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{1F1D4625-D39B-4428-A9DE-637A78BF9F19}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <definedNames>
     <definedName name="beta_t1">Original!$S$75:$S$77</definedName>
     <definedName name="beta_t2">Original!$S$60:$S$62</definedName>
@@ -164,9 +161,6 @@
     <t>double matrix: Exercise payoff value for each time and path #</t>
   </si>
   <si>
-    <t>Initiate the backward algorithm at maturity t=T=3 and calculate the option payoff, conditional on not exercising prior to maturity</t>
-  </si>
-  <si>
     <t>Path</t>
   </si>
   <si>
@@ -246,6 +240,9 @@
   </si>
   <si>
     <t>End of backward algorithm. We now simply discount the cash flows from their optimal exercise time and then take the average to get the price estimate</t>
+  </si>
+  <si>
+    <t>Initiate the backward algorithm and calculate the option payoff (exercise/intrinsic value), conditional on not exercising prior</t>
   </si>
 </sst>
 </file>
@@ -389,17 +386,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="2"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="3"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -410,6 +401,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="20% - Accent1" xfId="2" builtinId="30"/>
@@ -1864,155 +1861,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
-    <sheetNames>
-      <sheetName val="Sheet1"/>
-      <sheetName val="Sheet2"/>
-      <sheetName val="Sheet3"/>
-      <sheetName val="Original"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3">
-        <row r="10">
-          <cell r="B10">
-            <v>0</v>
-          </cell>
-          <cell r="C10">
-            <v>1</v>
-          </cell>
-          <cell r="D10">
-            <v>2</v>
-          </cell>
-          <cell r="E10">
-            <v>3</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="B11">
-            <v>1</v>
-          </cell>
-          <cell r="C11">
-            <v>1.0900000000000001</v>
-          </cell>
-          <cell r="D11">
-            <v>1.08</v>
-          </cell>
-          <cell r="E11">
-            <v>1.34</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="B12">
-            <v>1</v>
-          </cell>
-          <cell r="C12">
-            <v>1.1599999999999999</v>
-          </cell>
-          <cell r="D12">
-            <v>1.26</v>
-          </cell>
-          <cell r="E12">
-            <v>1.54</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="B13">
-            <v>1</v>
-          </cell>
-          <cell r="C13">
-            <v>1.22</v>
-          </cell>
-          <cell r="D13">
-            <v>1.07</v>
-          </cell>
-          <cell r="E13">
-            <v>1.03</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="B14">
-            <v>1</v>
-          </cell>
-          <cell r="C14">
-            <v>0.93</v>
-          </cell>
-          <cell r="D14">
-            <v>0.97</v>
-          </cell>
-          <cell r="E14">
-            <v>0.92</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="B15">
-            <v>1</v>
-          </cell>
-          <cell r="C15">
-            <v>1.1100000000000001</v>
-          </cell>
-          <cell r="D15">
-            <v>1.56</v>
-          </cell>
-          <cell r="E15">
-            <v>1.52</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="B16">
-            <v>1</v>
-          </cell>
-          <cell r="C16">
-            <v>0.76</v>
-          </cell>
-          <cell r="D16">
-            <v>0.77</v>
-          </cell>
-          <cell r="E16">
-            <v>0.9</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="B17">
-            <v>1</v>
-          </cell>
-          <cell r="C17">
-            <v>0.92</v>
-          </cell>
-          <cell r="D17">
-            <v>0.84</v>
-          </cell>
-          <cell r="E17">
-            <v>1.01</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="B18">
-            <v>1</v>
-          </cell>
-          <cell r="C18">
-            <v>0.88</v>
-          </cell>
-          <cell r="D18">
-            <v>1.22</v>
-          </cell>
-          <cell r="E18">
-            <v>1.34</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2332,8 +2180,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A6D6C7D-5047-4D1E-8F63-F2CFB597204C}">
   <dimension ref="A1:Z100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B88" sqref="B88"/>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="D66" sqref="D66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2382,36 +2230,36 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B10" s="4">
         <v>0</v>
       </c>
-      <c r="C10" s="5">
-        <v>1</v>
-      </c>
-      <c r="D10" s="5">
+      <c r="C10" s="4">
+        <v>1</v>
+      </c>
+      <c r="D10" s="4">
         <v>2</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="4">
         <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="5">
-        <v>1</v>
-      </c>
-      <c r="B11" s="6">
-        <f>S_0_0</f>
+      <c r="A11" s="4">
+        <v>1</v>
+      </c>
+      <c r="B11" s="5">
+        <f t="shared" ref="B11:B18" si="0">S_0_0</f>
         <v>1</v>
       </c>
       <c r="C11">
@@ -2425,11 +2273,11 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="5">
+      <c r="A12" s="4">
         <v>2</v>
       </c>
-      <c r="B12" s="6">
-        <f>S_0_0</f>
+      <c r="B12" s="5">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C12">
@@ -2443,11 +2291,11 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="5">
+      <c r="A13" s="4">
         <v>3</v>
       </c>
-      <c r="B13" s="6">
-        <f>S_0_0</f>
+      <c r="B13" s="5">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C13">
@@ -2461,11 +2309,11 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="5">
+      <c r="A14" s="4">
         <v>4</v>
       </c>
-      <c r="B14" s="6">
-        <f>S_0_0</f>
+      <c r="B14" s="5">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C14">
@@ -2479,11 +2327,11 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="5">
+      <c r="A15" s="4">
         <v>5</v>
       </c>
-      <c r="B15" s="6">
-        <f>S_0_0</f>
+      <c r="B15" s="5">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C15">
@@ -2497,11 +2345,11 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="5">
+      <c r="A16" s="4">
         <v>6</v>
       </c>
-      <c r="B16" s="6">
-        <f>S_0_0</f>
+      <c r="B16" s="5">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C16">
@@ -2515,11 +2363,11 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="5">
+      <c r="A17" s="4">
         <v>7</v>
       </c>
-      <c r="B17" s="6">
-        <f>S_0_0</f>
+      <c r="B17" s="5">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C17">
@@ -2533,11 +2381,11 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="5">
+      <c r="A18" s="4">
         <v>8</v>
       </c>
-      <c r="B18" s="6">
-        <f>S_0_0</f>
+      <c r="B18" s="5">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="C18">
@@ -2627,318 +2475,318 @@
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:5" s="7" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="1:5" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="32" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>27</v>
+        <v>54</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B34" s="18">
+      <c r="B34" s="16">
         <v>3</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B35" s="8" t="s">
+      <c r="B35" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="C35" s="8"/>
-      <c r="D35" s="8"/>
-      <c r="E35" s="8"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="18"/>
       <c r="G35" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="4" t="s">
+      <c r="A36" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B36" s="5">
+      <c r="B36" s="4">
         <v>0</v>
       </c>
-      <c r="C36" s="5">
-        <v>1</v>
-      </c>
-      <c r="D36" s="5">
+      <c r="C36" s="4">
+        <v>1</v>
+      </c>
+      <c r="D36" s="4">
         <v>2</v>
       </c>
-      <c r="E36" s="5">
+      <c r="E36" s="4">
         <v>3</v>
       </c>
       <c r="G36" s="1"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="5">
-        <v>1</v>
-      </c>
-      <c r="B37" s="6">
-        <f>MAX(0,STRIKE-B11)</f>
+      <c r="A37" s="4">
+        <v>1</v>
+      </c>
+      <c r="B37" s="5">
+        <f t="shared" ref="B37:D44" si="1">MAX(0,STRIKE-B11)</f>
         <v>0.10000000000000009</v>
       </c>
-      <c r="C37" s="6">
-        <f>MAX(0,STRIKE-C11)</f>
+      <c r="C37" s="5">
+        <f t="shared" si="1"/>
         <v>1.0000000000000009E-2</v>
       </c>
-      <c r="D37" s="6">
-        <f>MAX(0,STRIKE-D11)</f>
+      <c r="D37" s="5">
+        <f t="shared" si="1"/>
         <v>2.0000000000000018E-2</v>
       </c>
-      <c r="E37" s="6">
-        <f>MAX(0, STRIKE - E11)</f>
+      <c r="E37" s="5">
+        <f t="shared" ref="E37:E44" si="2">MAX(0, STRIKE - E11)</f>
         <v>0</v>
       </c>
-      <c r="G37" s="14">
+      <c r="G37" s="12">
         <v>3</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="5">
+      <c r="A38" s="4">
         <v>2</v>
       </c>
-      <c r="B38" s="6">
-        <f>MAX(0,STRIKE-B12)</f>
+      <c r="B38" s="5">
+        <f t="shared" si="1"/>
         <v>0.10000000000000009</v>
       </c>
-      <c r="C38" s="6">
-        <f>MAX(0,STRIKE-C12)</f>
+      <c r="C38" s="5">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="D38" s="6">
-        <f>MAX(0,STRIKE-D12)</f>
+      <c r="D38" s="5">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E38" s="6">
-        <f>MAX(0, STRIKE - E12)</f>
+      <c r="E38" s="5">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G38" s="15">
+      <c r="G38" s="13">
         <v>3</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="5">
+      <c r="A39" s="4">
         <v>3</v>
       </c>
-      <c r="B39" s="6">
-        <f>MAX(0,STRIKE-B13)</f>
+      <c r="B39" s="5">
+        <f t="shared" si="1"/>
         <v>0.10000000000000009</v>
       </c>
-      <c r="C39" s="6">
-        <f>MAX(0,STRIKE-C13)</f>
+      <c r="C39" s="5">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="D39" s="6">
-        <f>MAX(0,STRIKE-D13)</f>
+      <c r="D39" s="5">
+        <f t="shared" si="1"/>
         <v>3.0000000000000027E-2</v>
       </c>
-      <c r="E39" s="6">
-        <f>MAX(0, STRIKE - E13)</f>
+      <c r="E39" s="5">
+        <f t="shared" si="2"/>
         <v>7.0000000000000062E-2</v>
       </c>
-      <c r="G39" s="15">
+      <c r="G39" s="13">
         <v>3</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="5">
+      <c r="A40" s="4">
         <v>4</v>
       </c>
-      <c r="B40" s="6">
-        <f>MAX(0,STRIKE-B14)</f>
+      <c r="B40" s="5">
+        <f t="shared" si="1"/>
         <v>0.10000000000000009</v>
       </c>
-      <c r="C40" s="6">
-        <f>MAX(0,STRIKE-C14)</f>
+      <c r="C40" s="5">
+        <f t="shared" si="1"/>
         <v>0.17000000000000004</v>
       </c>
-      <c r="D40" s="6">
-        <f>MAX(0,STRIKE-D14)</f>
+      <c r="D40" s="5">
+        <f t="shared" si="1"/>
         <v>0.13000000000000012</v>
       </c>
-      <c r="E40" s="6">
-        <f>MAX(0, STRIKE - E14)</f>
+      <c r="E40" s="5">
+        <f t="shared" si="2"/>
         <v>0.18000000000000005</v>
       </c>
-      <c r="G40" s="15">
+      <c r="G40" s="13">
         <v>3</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="5">
+      <c r="A41" s="4">
         <v>5</v>
       </c>
-      <c r="B41" s="6">
-        <f>MAX(0,STRIKE-B15)</f>
+      <c r="B41" s="5">
+        <f t="shared" si="1"/>
         <v>0.10000000000000009</v>
       </c>
-      <c r="C41" s="6">
-        <f>MAX(0,STRIKE-C15)</f>
+      <c r="C41" s="5">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="D41" s="6">
-        <f>MAX(0,STRIKE-D15)</f>
+      <c r="D41" s="5">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E41" s="6">
-        <f>MAX(0, STRIKE - E15)</f>
+      <c r="E41" s="5">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G41" s="15">
+      <c r="G41" s="13">
         <v>3</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="5">
+      <c r="A42" s="4">
         <v>6</v>
       </c>
-      <c r="B42" s="6">
-        <f>MAX(0,STRIKE-B16)</f>
+      <c r="B42" s="5">
+        <f t="shared" si="1"/>
         <v>0.10000000000000009</v>
       </c>
-      <c r="C42" s="6">
-        <f>MAX(0,STRIKE-C16)</f>
+      <c r="C42" s="5">
+        <f t="shared" si="1"/>
         <v>0.34000000000000008</v>
       </c>
-      <c r="D42" s="6">
-        <f>MAX(0,STRIKE-D16)</f>
+      <c r="D42" s="5">
+        <f t="shared" si="1"/>
         <v>0.33000000000000007</v>
       </c>
-      <c r="E42" s="6">
-        <f>MAX(0, STRIKE - E16)</f>
+      <c r="E42" s="5">
+        <f t="shared" si="2"/>
         <v>0.20000000000000007</v>
       </c>
-      <c r="G42" s="15">
+      <c r="G42" s="13">
         <v>3</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="5">
+      <c r="A43" s="4">
         <v>7</v>
       </c>
-      <c r="B43" s="6">
-        <f>MAX(0,STRIKE-B17)</f>
+      <c r="B43" s="5">
+        <f t="shared" si="1"/>
         <v>0.10000000000000009</v>
       </c>
-      <c r="C43" s="6">
-        <f>MAX(0,STRIKE-C17)</f>
+      <c r="C43" s="5">
+        <f t="shared" si="1"/>
         <v>0.18000000000000005</v>
       </c>
-      <c r="D43" s="6">
-        <f>MAX(0,STRIKE-D17)</f>
+      <c r="D43" s="5">
+        <f t="shared" si="1"/>
         <v>0.26000000000000012</v>
       </c>
-      <c r="E43" s="6">
-        <f>MAX(0, STRIKE - E17)</f>
+      <c r="E43" s="5">
+        <f t="shared" si="2"/>
         <v>9.000000000000008E-2</v>
       </c>
-      <c r="G43" s="15">
+      <c r="G43" s="13">
         <v>3</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="5">
+      <c r="A44" s="4">
         <v>8</v>
       </c>
-      <c r="B44" s="6">
-        <f>MAX(0,STRIKE-B18)</f>
+      <c r="B44" s="5">
+        <f t="shared" si="1"/>
         <v>0.10000000000000009</v>
       </c>
-      <c r="C44" s="6">
-        <f>MAX(0,STRIKE-C18)</f>
+      <c r="C44" s="5">
+        <f t="shared" si="1"/>
         <v>0.22000000000000008</v>
       </c>
-      <c r="D44" s="6">
-        <f>MAX(0,STRIKE-D18)</f>
+      <c r="D44" s="5">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E44" s="6">
-        <f>MAX(0, STRIKE - E18)</f>
+      <c r="E44" s="5">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G44" s="16">
+      <c r="G44" s="14">
         <v>3</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E45" s="6"/>
-    </row>
-    <row r="46" spans="1:7" s="7" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E46" s="9"/>
+      <c r="E45" s="5"/>
+    </row>
+    <row r="46" spans="1:7" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E46" s="7"/>
     </row>
     <row r="47" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="E47" s="6"/>
+      <c r="E47" s="5"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="49" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A49" s="8" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="49" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A49" s="10" t="s">
+      <c r="B49" t="s">
         <v>30</v>
       </c>
-      <c r="B49" t="s">
+    </row>
+    <row r="50" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A50" s="8" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="50" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A50" s="10" t="s">
+      <c r="B50" t="s">
         <v>32</v>
       </c>
-      <c r="B50" t="s">
+    </row>
+    <row r="51" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A51" s="8" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="51" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A51" s="10" t="s">
+      <c r="B51" t="s">
         <v>34</v>
       </c>
-      <c r="B51" t="s">
+    </row>
+    <row r="52" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A52" s="8" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="52" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A52" s="10" t="s">
+      <c r="B52" t="s">
         <v>36</v>
       </c>
-      <c r="B52" t="s">
+    </row>
+    <row r="53" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A53" s="8" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="53" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A53" s="10" t="s">
+      <c r="B53" t="s">
         <v>38</v>
       </c>
-      <c r="B53" t="s">
+    </row>
+    <row r="54" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A54" s="8" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="54" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A54" s="10" t="s">
+      <c r="B54" t="s">
         <v>40</v>
       </c>
-      <c r="B54" t="s">
+    </row>
+    <row r="55" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A55" s="8" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="55" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A55" s="10" t="s">
+      <c r="B55" t="s">
         <v>42</v>
-      </c>
-      <c r="B55" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="56" spans="1:26" x14ac:dyDescent="0.25">
       <c r="H56" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y56" t="s">
         <v>44</v>
-      </c>
-      <c r="Y56" t="s">
-        <v>45</v>
       </c>
       <c r="Z56">
         <f>COUNT(L60:L67)</f>
@@ -2949,39 +2797,39 @@
       <c r="A57" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B57" s="18">
+      <c r="B57" s="16">
         <v>2</v>
       </c>
     </row>
     <row r="58" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="D58" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="F58" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="H58" s="10" t="s">
-        <v>34</v>
+      <c r="D58" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F58" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H58" s="8" t="s">
+        <v>33</v>
       </c>
       <c r="M58" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q58" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="S58" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="U58" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="Z58" s="10" t="s">
-        <v>42</v>
+        <v>45</v>
+      </c>
+      <c r="Q58" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="S58" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="U58" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z58" s="8" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="59" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>13</v>
@@ -2990,37 +2838,37 @@
         <v>15</v>
       </c>
       <c r="H59" t="s">
+        <v>46</v>
+      </c>
+      <c r="I59" t="s">
         <v>47</v>
       </c>
-      <c r="I59" t="s">
+      <c r="J59" t="s">
         <v>48</v>
-      </c>
-      <c r="J59" t="s">
-        <v>49</v>
       </c>
       <c r="L59" t="s">
         <v>3</v>
       </c>
       <c r="M59" t="s">
+        <v>49</v>
+      </c>
+      <c r="N59" t="s">
+        <v>47</v>
+      </c>
+      <c r="O59" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q59" t="s">
         <v>50</v>
-      </c>
-      <c r="N59" t="s">
-        <v>48</v>
-      </c>
-      <c r="O59" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q59" t="s">
-        <v>51</v>
       </c>
       <c r="S59" t="s">
         <v>21</v>
       </c>
       <c r="U59" t="s">
+        <v>51</v>
+      </c>
+      <c r="W59" t="s">
         <v>52</v>
-      </c>
-      <c r="W59" t="s">
-        <v>53</v>
       </c>
       <c r="X59" s="1" t="s">
         <v>11</v>
@@ -3030,10 +2878,10 @@
       </c>
     </row>
     <row r="60" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A60" s="5">
-        <v>1</v>
-      </c>
-      <c r="D60" s="11" cm="1">
+      <c r="A60" s="4">
+        <v>1</v>
+      </c>
+      <c r="D60" s="9" cm="1">
         <f t="array" ref="D60:D67">EXP(-RISKFREE*1)*payoff_t3</f>
         <v>0</v>
       </c>
@@ -3052,7 +2900,7 @@
         <f t="array" ref="J60:J67">S_t2^2</f>
         <v>1.1664000000000001</v>
       </c>
-      <c r="L60" s="5" cm="1">
+      <c r="L60" s="4" cm="1">
         <f t="array" ref="L60:L64">_xlfn._xlws.FILTER(A60:A67,F60:F67)</f>
         <v>1</v>
       </c>
@@ -3068,15 +2916,15 @@
         <f t="array" ref="O60:O64">_xlfn._xlws.FILTER(J60:J67,F60:F67)</f>
         <v>1.1664000000000001</v>
       </c>
-      <c r="Q60" s="11" cm="1">
+      <c r="Q60" s="9" cm="1">
         <f t="array" ref="Q60:Q64">_xlfn._xlws.FILTER(D60:D67,F60:F67)</f>
         <v>0</v>
       </c>
-      <c r="S60" s="14" cm="1">
+      <c r="S60" s="12" cm="1">
         <f t="array" ref="S60:S62">MMULT(MINVERSE(MMULT(TRANSPOSE(X_t2),X_t2)),MMULT(TRANSPOSE(X_t2),Y_t2))</f>
         <v>-1.0699876552821479</v>
       </c>
-      <c r="U60" s="11" cm="1">
+      <c r="U60" s="9" cm="1">
         <f t="array" ref="U60:U64">MMULT(X_t2,beta_t2)</f>
         <v>3.6740560851308501E-2</v>
       </c>
@@ -3088,16 +2936,16 @@
         <f>IF(W60&gt;U60,t_2,0)</f>
         <v>0</v>
       </c>
-      <c r="Z60" s="12">
-        <f>_xlfn.IFNA(IF(VLOOKUP(A60,$L$60:$X$64,13,FALSE)=t_2,t_2,G37),G37)</f>
+      <c r="Z60" s="10">
+        <f t="shared" ref="Z60:Z67" si="3">_xlfn.IFNA(IF(VLOOKUP(A60,$L$60:$X$64,13,FALSE)=t_2,t_2,G37),G37)</f>
         <v>3</v>
       </c>
     </row>
     <row r="61" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A61" s="5">
+      <c r="A61" s="4">
         <v>2</v>
       </c>
-      <c r="D61" s="11">
+      <c r="D61" s="9">
         <v>0</v>
       </c>
       <c r="F61">
@@ -3112,7 +2960,7 @@
       <c r="J61">
         <v>1.5876000000000001</v>
       </c>
-      <c r="L61" s="5">
+      <c r="L61" s="4">
         <v>3</v>
       </c>
       <c r="M61">
@@ -3124,13 +2972,13 @@
       <c r="O61">
         <v>1.1449</v>
       </c>
-      <c r="Q61" s="11">
+      <c r="Q61" s="9">
         <v>6.5923517350897465E-2</v>
       </c>
-      <c r="S61" s="15">
+      <c r="S61" s="13">
         <v>2.983410625839042</v>
       </c>
-      <c r="U61" s="11">
+      <c r="U61" s="9">
         <v>4.5898342525971358E-2</v>
       </c>
       <c r="W61">
@@ -3141,16 +2989,16 @@
         <f>IF(W61&gt;U61,t_2,0)</f>
         <v>0</v>
       </c>
-      <c r="Z61" s="12">
-        <f>_xlfn.IFNA(IF(VLOOKUP(A61,$L$60:$X$64,13,FALSE)=t_2,t_2,G38),G38)</f>
+      <c r="Z61" s="10">
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
     </row>
     <row r="62" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="5">
+      <c r="A62" s="4">
         <v>3</v>
       </c>
-      <c r="D62" s="11">
+      <c r="D62" s="9">
         <v>6.5923517350897465E-2</v>
       </c>
       <c r="F62">
@@ -3165,7 +3013,7 @@
       <c r="J62">
         <v>1.1449</v>
       </c>
-      <c r="L62" s="5">
+      <c r="L62" s="4">
         <v>4</v>
       </c>
       <c r="M62">
@@ -3177,13 +3025,13 @@
       <c r="O62">
         <v>0.94089999999999996</v>
       </c>
-      <c r="Q62" s="11">
+      <c r="Q62" s="9">
         <v>0.16951761604516483</v>
       </c>
-      <c r="S62" s="16">
+      <c r="S62" s="14">
         <v>-1.8135761829327066</v>
       </c>
-      <c r="U62" s="11">
+      <c r="U62" s="9">
         <v>0.11752682126033953</v>
       </c>
       <c r="W62">
@@ -3194,16 +3042,16 @@
         <f>IF(W62&gt;U62,t_2,0)</f>
         <v>2</v>
       </c>
-      <c r="Z62" s="12">
-        <f>_xlfn.IFNA(IF(VLOOKUP(A62,$L$60:$X$64,13,FALSE)=t_2,t_2,G39),G39)</f>
+      <c r="Z62" s="10">
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
     </row>
     <row r="63" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A63" s="5">
+      <c r="A63" s="4">
         <v>4</v>
       </c>
-      <c r="D63" s="11">
+      <c r="D63" s="9">
         <v>0.16951761604516483</v>
       </c>
       <c r="F63">
@@ -3218,7 +3066,7 @@
       <c r="J63">
         <v>0.94089999999999996</v>
       </c>
-      <c r="L63" s="5">
+      <c r="L63" s="4">
         <v>6</v>
       </c>
       <c r="M63">
@@ -3230,10 +3078,10 @@
       <c r="O63">
         <v>0.59289999999999998</v>
       </c>
-      <c r="Q63" s="11">
+      <c r="Q63" s="9">
         <v>0.18835290671684982</v>
       </c>
-      <c r="U63" s="11">
+      <c r="U63" s="9">
         <v>0.15196920775311273</v>
       </c>
       <c r="W63">
@@ -3244,16 +3092,16 @@
         <f>IF(W63&gt;U63,t_2,0)</f>
         <v>2</v>
       </c>
-      <c r="Z63" s="12">
-        <f>_xlfn.IFNA(IF(VLOOKUP(A63,$L$60:$X$64,13,FALSE)=t_2,t_2,G40),G40)</f>
+      <c r="Z63" s="10">
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
     </row>
     <row r="64" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A64" s="5">
+      <c r="A64" s="4">
         <v>5</v>
       </c>
-      <c r="D64" s="11">
+      <c r="D64" s="9">
         <v>0</v>
       </c>
       <c r="F64">
@@ -3268,7 +3116,7 @@
       <c r="J64">
         <v>2.4336000000000002</v>
       </c>
-      <c r="L64" s="5">
+      <c r="L64" s="4">
         <v>7</v>
       </c>
       <c r="M64">
@@ -3280,10 +3128,10 @@
       <c r="O64">
         <v>0.70559999999999989</v>
       </c>
-      <c r="Q64" s="11">
+      <c r="Q64" s="9">
         <v>8.4758808022582455E-2</v>
       </c>
-      <c r="U64" s="11">
+      <c r="U64" s="9">
         <v>0.15641791574532982</v>
       </c>
       <c r="W64">
@@ -3294,16 +3142,16 @@
         <f>IF(W64&gt;U64,t_2,0)</f>
         <v>2</v>
       </c>
-      <c r="Z64" s="12">
-        <f>_xlfn.IFNA(IF(VLOOKUP(A64,$L$60:$X$64,13,FALSE)=t_2,t_2,G41),G41)</f>
+      <c r="Z64" s="10">
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
     </row>
     <row r="65" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A65" s="5">
+      <c r="A65" s="4">
         <v>6</v>
       </c>
-      <c r="D65" s="11">
+      <c r="D65" s="9">
         <v>0.18835290671684982</v>
       </c>
       <c r="F65">
@@ -3318,16 +3166,16 @@
       <c r="J65">
         <v>0.59289999999999998</v>
       </c>
-      <c r="Z65" s="12">
-        <f>_xlfn.IFNA(IF(VLOOKUP(A65,$L$60:$X$64,13,FALSE)=t_2,t_2,G42),G42)</f>
+      <c r="Z65" s="10">
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
     </row>
     <row r="66" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A66" s="5">
+      <c r="A66" s="4">
         <v>7</v>
       </c>
-      <c r="D66" s="11">
+      <c r="D66" s="9">
         <v>8.4758808022582455E-2</v>
       </c>
       <c r="F66">
@@ -3342,16 +3190,16 @@
       <c r="J66">
         <v>0.70559999999999989</v>
       </c>
-      <c r="Z66" s="12">
-        <f>_xlfn.IFNA(IF(VLOOKUP(A66,$L$60:$X$64,13,FALSE)=t_2,t_2,G43),G43)</f>
+      <c r="Z66" s="10">
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
     </row>
     <row r="67" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A67" s="5">
+      <c r="A67" s="4">
         <v>8</v>
       </c>
-      <c r="D67" s="11">
+      <c r="D67" s="9">
         <v>0</v>
       </c>
       <c r="F67">
@@ -3366,26 +3214,26 @@
       <c r="J67">
         <v>1.4883999999999999</v>
       </c>
-      <c r="Z67" s="12">
-        <f>_xlfn.IFNA(IF(VLOOKUP(A67,$L$60:$X$64,13,FALSE)=t_2,t_2,G44),G44)</f>
+      <c r="Z67" s="10">
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
     </row>
     <row r="68" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="Z68" s="12"/>
-    </row>
-    <row r="69" spans="1:26" s="7" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="Z69" s="13"/>
+      <c r="Z68" s="10"/>
+    </row>
+    <row r="69" spans="1:26" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z69" s="11"/>
     </row>
     <row r="70" spans="1:26" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="Z70" s="12"/>
+      <c r="Z70" s="10"/>
     </row>
     <row r="71" spans="1:26" x14ac:dyDescent="0.25">
       <c r="H71" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y71" t="s">
         <v>44</v>
-      </c>
-      <c r="Y71" t="s">
-        <v>45</v>
       </c>
       <c r="Z71">
         <f>COUNT(L75:L82)</f>
@@ -3396,39 +3244,39 @@
       <c r="A72" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B72" s="18">
+      <c r="B72" s="16">
         <v>1</v>
       </c>
     </row>
     <row r="73" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="C73" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="F73" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="H73" s="10" t="s">
-        <v>34</v>
+      <c r="C73" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F73" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H73" s="8" t="s">
+        <v>33</v>
       </c>
       <c r="M73" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q73" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="S73" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="U73" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="Z73" s="10" t="s">
-        <v>42</v>
+        <v>45</v>
+      </c>
+      <c r="Q73" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="S73" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="U73" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z73" s="8" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="74" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>13</v>
@@ -3437,37 +3285,37 @@
         <v>15</v>
       </c>
       <c r="H74" t="s">
+        <v>46</v>
+      </c>
+      <c r="I74" t="s">
         <v>47</v>
       </c>
-      <c r="I74" t="s">
+      <c r="J74" t="s">
         <v>48</v>
-      </c>
-      <c r="J74" t="s">
-        <v>49</v>
       </c>
       <c r="L74" t="s">
         <v>3</v>
       </c>
       <c r="M74" t="s">
+        <v>49</v>
+      </c>
+      <c r="N74" t="s">
+        <v>47</v>
+      </c>
+      <c r="O74" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q74" t="s">
         <v>50</v>
-      </c>
-      <c r="N74" t="s">
-        <v>48</v>
-      </c>
-      <c r="O74" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q74" t="s">
-        <v>51</v>
       </c>
       <c r="S74" t="s">
         <v>21</v>
       </c>
       <c r="U74" t="s">
+        <v>51</v>
+      </c>
+      <c r="W74" t="s">
         <v>52</v>
-      </c>
-      <c r="W74" t="s">
-        <v>53</v>
       </c>
       <c r="X74" s="1" t="s">
         <v>11</v>
@@ -3477,11 +3325,11 @@
       </c>
     </row>
     <row r="75" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A75" s="5">
-        <v>1</v>
-      </c>
-      <c r="C75" s="11">
-        <f>EXP(-RISKFREE*(Z60-$B$72))*IF(Z60=3,E37,D37)</f>
+      <c r="A75" s="4">
+        <v>1</v>
+      </c>
+      <c r="C75" s="9">
+        <f t="shared" ref="C75:C82" si="4">EXP(-RISKFREE*(Z60-$B$72))*IF(Z60=3,E37,D37)</f>
         <v>0</v>
       </c>
       <c r="F75">
@@ -3499,7 +3347,7 @@
         <f t="array" ref="J75:J82">S_t1^2</f>
         <v>1.1881000000000002</v>
       </c>
-      <c r="L75" s="5" cm="1">
+      <c r="L75" s="4" cm="1">
         <f t="array" ref="L75:L79">_xlfn._xlws.FILTER(A75:A82,F75:F82)</f>
         <v>1</v>
       </c>
@@ -3515,15 +3363,15 @@
         <f t="array" ref="O75:O79">_xlfn._xlws.FILTER(J75:J82,F75:F82)</f>
         <v>1.1881000000000002</v>
       </c>
-      <c r="Q75" s="11" cm="1">
+      <c r="Q75" s="9" cm="1">
         <f t="array" ref="Q75:Q79">_xlfn._xlws.FILTER(C75:C82,F75:F82)</f>
         <v>0</v>
       </c>
-      <c r="S75" s="14">
+      <c r="S75" s="12">
         <f t="array" ref="S75:S77">MMULT(MINVERSE(MMULT(TRANSPOSE(X_t1),X_t1)),MMULT(TRANSPOSE(X_t1),Y_t1))</f>
         <v>2.0375123423771129</v>
       </c>
-      <c r="U75" s="11" cm="1">
+      <c r="U75" s="9" cm="1">
         <f t="array" ref="U75:U79">MMULT(X_t1,beta_t1)</f>
         <v>1.3485105283447041E-2</v>
       </c>
@@ -3535,17 +3383,17 @@
         <f t="array" ref="X75">IF(W75&gt;U75,t_1,0)</f>
         <v>0</v>
       </c>
-      <c r="Z75" s="12">
-        <f>_xlfn.IFNA(IF(VLOOKUP(A60,$L$75:$X$79,13,FALSE)=t_1,t_1,Z60),Z60)</f>
+      <c r="Z75" s="10">
+        <f t="shared" ref="Z75:Z82" si="5">_xlfn.IFNA(IF(VLOOKUP(A60,$L$75:$X$79,13,FALSE)=t_1,t_1,Z60),Z60)</f>
         <v>3</v>
       </c>
     </row>
     <row r="76" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A76" s="5">
+      <c r="A76" s="4">
         <v>2</v>
       </c>
-      <c r="C76" s="11">
-        <f>EXP(-RISKFREE*(Z61-$B$72))*IF(Z61=3,E38,D38)</f>
+      <c r="C76" s="9">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F76">
@@ -3560,7 +3408,7 @@
       <c r="J76">
         <v>1.3455999999999999</v>
       </c>
-      <c r="L76" s="5">
+      <c r="L76" s="4">
         <v>4</v>
       </c>
       <c r="M76">
@@ -3572,13 +3420,13 @@
       <c r="O76">
         <v>0.86490000000000011</v>
       </c>
-      <c r="Q76" s="11">
+      <c r="Q76" s="9">
         <v>0.12242938936595245</v>
       </c>
-      <c r="S76" s="15">
+      <c r="S76" s="13">
         <v>-3.3354434031348319</v>
       </c>
-      <c r="U76" s="11">
+      <c r="U76" s="9">
         <v>0.10874928051064026</v>
       </c>
       <c r="W76">
@@ -3588,17 +3436,17 @@
         <f t="array" ref="X76">IF(W76&gt;U76,t_1,0)</f>
         <v>1</v>
       </c>
-      <c r="Z76" s="12">
-        <f>_xlfn.IFNA(IF(VLOOKUP(A61,$L$75:$X$79,13,FALSE)=t_1,t_1,Z61),Z61)</f>
+      <c r="Z76" s="10">
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
     </row>
     <row r="77" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="5">
+      <c r="A77" s="4">
         <v>3</v>
       </c>
-      <c r="C77" s="11">
-        <f>EXP(-RISKFREE*(Z62-$B$72))*IF(Z62=3,E39,D39)</f>
+      <c r="C77" s="9">
+        <f t="shared" si="4"/>
         <v>6.2084430570201077E-2</v>
       </c>
       <c r="F77">
@@ -3613,7 +3461,7 @@
       <c r="J77">
         <v>1.4883999999999999</v>
       </c>
-      <c r="L77" s="5">
+      <c r="L77" s="4">
         <v>6</v>
       </c>
       <c r="M77">
@@ -3625,13 +3473,13 @@
       <c r="O77">
         <v>0.5776</v>
       </c>
-      <c r="Q77" s="11">
+      <c r="Q77" s="9">
         <v>0.31078229608280217</v>
       </c>
-      <c r="S77" s="16">
+      <c r="S77" s="14">
         <v>1.3564565881014232</v>
       </c>
-      <c r="U77" s="11">
+      <c r="U77" s="9">
         <v>0.28606468128202267</v>
       </c>
       <c r="W77">
@@ -3641,17 +3489,17 @@
         <f t="array" ref="X77">IF(W77&gt;U77,t_1,0)</f>
         <v>1</v>
       </c>
-      <c r="Z77" s="12">
-        <f>_xlfn.IFNA(IF(VLOOKUP(A62,$L$75:$X$79,13,FALSE)=t_1,t_1,Z62),Z62)</f>
+      <c r="Z77" s="10">
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
     </row>
     <row r="78" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A78" s="5">
+      <c r="A78" s="4">
         <v>4</v>
       </c>
-      <c r="C78" s="11">
-        <f>EXP(-RISKFREE*(Z63-$B$72))*IF(Z63=3,E40,D40)</f>
+      <c r="C78" s="9">
+        <f t="shared" si="4"/>
         <v>0.12242938936595245</v>
       </c>
       <c r="F78">
@@ -3666,7 +3514,7 @@
       <c r="J78">
         <v>0.86490000000000011</v>
       </c>
-      <c r="L78" s="5">
+      <c r="L78" s="4">
         <v>7</v>
       </c>
       <c r="M78">
@@ -3678,10 +3526,10 @@
       <c r="O78">
         <v>0.84640000000000004</v>
       </c>
-      <c r="Q78" s="11">
+      <c r="Q78" s="9">
         <v>0.24485877873190479</v>
       </c>
-      <c r="U78" s="11">
+      <c r="U78" s="9">
         <v>0.11700926766211195</v>
       </c>
       <c r="W78">
@@ -3691,17 +3539,17 @@
         <f t="array" ref="X78">IF(W78&gt;U78,t_1,0)</f>
         <v>1</v>
       </c>
-      <c r="Z78" s="12">
-        <f>_xlfn.IFNA(IF(VLOOKUP(A63,$L$75:$X$79,13,FALSE)=t_1,t_1,Z63),Z63)</f>
+      <c r="Z78" s="10">
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
     <row r="79" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A79" s="5">
+      <c r="A79" s="4">
         <v>5</v>
       </c>
-      <c r="C79" s="11">
-        <f>EXP(-RISKFREE*(Z64-$B$72))*IF(Z64=3,E41,D41)</f>
+      <c r="C79" s="9">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F79">
@@ -3716,7 +3564,7 @@
       <c r="J79">
         <v>1.2321000000000002</v>
       </c>
-      <c r="L79" s="5">
+      <c r="L79" s="4">
         <v>8</v>
       </c>
       <c r="M79">
@@ -3728,10 +3576,10 @@
       <c r="O79">
         <v>0.77439999999999998</v>
       </c>
-      <c r="Q79" s="11">
+      <c r="Q79" s="9">
         <v>0</v>
       </c>
-      <c r="U79" s="11">
+      <c r="U79" s="9">
         <v>0.15276212944420275</v>
       </c>
       <c r="W79">
@@ -3741,17 +3589,17 @@
         <f t="array" ref="X79">IF(W79&gt;U79,t_1,0)</f>
         <v>1</v>
       </c>
-      <c r="Z79" s="12">
-        <f>_xlfn.IFNA(IF(VLOOKUP(A64,$L$75:$X$79,13,FALSE)=t_1,t_1,Z64),Z64)</f>
+      <c r="Z79" s="10">
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
     </row>
     <row r="80" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A80" s="5">
+      <c r="A80" s="4">
         <v>6</v>
       </c>
-      <c r="C80" s="11">
-        <f>EXP(-RISKFREE*(Z65-$B$72))*IF(Z65=3,E42,D42)</f>
+      <c r="C80" s="9">
+        <f t="shared" si="4"/>
         <v>0.31078229608280217</v>
       </c>
       <c r="F80">
@@ -3766,17 +3614,17 @@
       <c r="J80">
         <v>0.5776</v>
       </c>
-      <c r="Z80" s="12">
-        <f>_xlfn.IFNA(IF(VLOOKUP(A65,$L$75:$X$79,13,FALSE)=t_1,t_1,Z65),Z65)</f>
+      <c r="Z80" s="10">
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
     <row r="81" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A81" s="5">
+      <c r="A81" s="4">
         <v>7</v>
       </c>
-      <c r="C81" s="11">
-        <f>EXP(-RISKFREE*(Z66-$B$72))*IF(Z66=3,E43,D43)</f>
+      <c r="C81" s="9">
+        <f t="shared" si="4"/>
         <v>0.24485877873190479</v>
       </c>
       <c r="F81">
@@ -3791,17 +3639,17 @@
       <c r="J81">
         <v>0.84640000000000004</v>
       </c>
-      <c r="Z81" s="12">
-        <f>_xlfn.IFNA(IF(VLOOKUP(A66,$L$75:$X$79,13,FALSE)=t_1,t_1,Z66),Z66)</f>
+      <c r="Z81" s="10">
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
     <row r="82" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A82" s="5">
+      <c r="A82" s="4">
         <v>8</v>
       </c>
-      <c r="C82" s="11">
-        <f>EXP(-RISKFREE*(Z67-$B$72))*IF(Z67=3,E44,D44)</f>
+      <c r="C82" s="9">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F82">
@@ -3816,127 +3664,127 @@
       <c r="J82">
         <v>0.77439999999999998</v>
       </c>
-      <c r="Z82" s="12">
-        <f>_xlfn.IFNA(IF(VLOOKUP(A67,$L$75:$X$79,13,FALSE)=t_1,t_1,Z67),Z67)</f>
+      <c r="Z82" s="10">
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
     <row r="83" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="C83" s="11"/>
+      <c r="C83" s="9"/>
     </row>
     <row r="84" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="C84" s="11"/>
-      <c r="Z84" s="12"/>
-    </row>
-    <row r="85" spans="1:26" s="7" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="Z85" s="13"/>
+      <c r="C84" s="9"/>
+      <c r="Z84" s="10"/>
+    </row>
+    <row r="85" spans="1:26" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Z85" s="11"/>
     </row>
     <row r="86" spans="1:26" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="Z86" s="12"/>
+      <c r="Z86" s="10"/>
     </row>
     <row r="87" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="88" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B88" s="18">
+      <c r="B88" s="16">
         <v>0</v>
       </c>
     </row>
     <row r="89" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="B89" s="10" t="s">
-        <v>30</v>
+      <c r="B89" s="8" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="90" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="91" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A91" s="5">
-        <v>1</v>
-      </c>
-      <c r="B91" s="11">
-        <f>EXP(-RISKFREE*(Z75-$B$88))*IF(Z75=3,E37,IF(Z75=2,D37,C37))</f>
+      <c r="A91" s="4">
+        <v>1</v>
+      </c>
+      <c r="B91" s="9">
+        <f t="shared" ref="B91:B98" si="6">EXP(-RISKFREE*(Z75-$B$88))*IF(Z75=3,E37,IF(Z75=2,D37,C37))</f>
         <v>0</v>
       </c>
     </row>
     <row r="92" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A92" s="5">
+      <c r="A92" s="4">
         <v>2</v>
       </c>
-      <c r="B92" s="11">
-        <f>EXP(-RISKFREE*(Z76-$B$88))*IF(Z76=3,E38,IF(Z76=2,D38,C38))</f>
+      <c r="B92" s="9">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="93" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A93" s="5">
+      <c r="A93" s="4">
         <v>3</v>
       </c>
-      <c r="B93" s="11">
-        <f>EXP(-RISKFREE*(Z77-$B$88))*IF(Z77=3,E39,IF(Z77=2,D39,C39))</f>
+      <c r="B93" s="9">
+        <f t="shared" si="6"/>
         <v>5.8468914798789094E-2</v>
       </c>
     </row>
     <row r="94" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A94" s="5">
+      <c r="A94" s="4">
         <v>4</v>
       </c>
-      <c r="B94" s="11">
-        <f>EXP(-RISKFREE*(Z78-$B$88))*IF(Z78=3,E40,IF(Z78=2,D40,C40))</f>
+      <c r="B94" s="9">
+        <f t="shared" si="6"/>
         <v>0.16009997070932233</v>
       </c>
     </row>
     <row r="95" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A95" s="5">
+      <c r="A95" s="4">
         <v>5</v>
       </c>
-      <c r="B95" s="11">
-        <f>EXP(-RISKFREE*(Z79-$B$88))*IF(Z79=3,E41,IF(Z79=2,D41,C41))</f>
+      <c r="B95" s="9">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
     <row r="96" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A96" s="5">
+      <c r="A96" s="4">
         <v>6</v>
       </c>
-      <c r="B96" s="11">
-        <f>EXP(-RISKFREE*(Z80-$B$88))*IF(Z80=3,E42,IF(Z80=2,D42,C42))</f>
+      <c r="B96" s="9">
+        <f t="shared" si="6"/>
         <v>0.32019994141864466</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97" s="5">
+      <c r="A97" s="4">
         <v>7</v>
       </c>
-      <c r="B97" s="11">
-        <f>EXP(-RISKFREE*(Z81-$B$88))*IF(Z81=3,E43,IF(Z81=2,D43,C43))</f>
+      <c r="B97" s="9">
+        <f t="shared" si="6"/>
         <v>0.16951761604516483</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98" s="5">
+      <c r="A98" s="4">
         <v>8</v>
       </c>
-      <c r="B98" s="11">
-        <f>EXP(-RISKFREE*(Z82-$B$88))*IF(Z82=3,E44,IF(Z82=2,D44,C44))</f>
+      <c r="B98" s="9">
+        <f t="shared" si="6"/>
         <v>0.20718819738853481</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B99" s="11"/>
+      <c r="B99" s="9"/>
     </row>
     <row r="100" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B100" s="17">
+      <c r="B100" s="15">
         <f>AVERAGE(B91:B98)</f>
         <v>0.11443433004505696</v>
       </c>
@@ -3947,6 +3795,7 @@
     <mergeCell ref="B35:E35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>